<commit_message>
Fix typo "ex tune" to "ex tunc"
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - Latein - Fachvokabular Jus (JKU, Austria).xlsx
+++ b/flashcards/Memcode - Latein - Fachvokabular Jus (JKU, Austria).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C64D4A4-60D9-4398-B6E5-E3D9D76D5359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E00706C-313A-43E6-BD83-AB9069B35016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="390" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latein - Fachvokabular Rechtswi" sheetId="1" r:id="rId1"/>
@@ -4298,9 +4298,6 @@
     <t>aus einer verwerflichen Sache entsteht keine Klage</t>
   </si>
   <si>
-    <t>ex tune</t>
-  </si>
-  <si>
     <t>vom damaligen Zeitpunkt an</t>
   </si>
   <si>
@@ -6529,6 +6526,9 @@
   </si>
   <si>
     <t>omnis definitio in iure civile periculosa est</t>
+  </si>
+  <si>
+    <t>ex tunc</t>
   </si>
 </sst>
 </file>
@@ -6922,8 +6922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1086"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="B261" sqref="B261"/>
+    <sheetView tabSelected="1" topLeftCell="A713" workbookViewId="0">
+      <selection activeCell="A721" sqref="A721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +6997,7 @@
     </row>
     <row r="9" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
@@ -9005,7 +9005,7 @@
     </row>
     <row r="260" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>516</v>
@@ -9016,7 +9016,7 @@
         <v>517</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="262" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -9981,10 +9981,10 @@
     </row>
     <row r="382" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B382" s="2" t="s">
         <v>2163</v>
-      </c>
-      <c r="B382" s="2" t="s">
-        <v>2164</v>
       </c>
     </row>
     <row r="383" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -10005,10 +10005,10 @@
     </row>
     <row r="385" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B385" s="2" t="s">
         <v>2161</v>
-      </c>
-      <c r="B385" s="2" t="s">
-        <v>2162</v>
       </c>
     </row>
     <row r="386" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -10136,7 +10136,7 @@
         <v>791</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="402" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -12685,2599 +12685,2599 @@
     </row>
     <row r="720" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A720" s="2" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B720" s="2" t="s">
         <v>1427</v>
-      </c>
-      <c r="B720" s="2" t="s">
-        <v>1428</v>
       </c>
     </row>
     <row r="721" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A721" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B721" s="2" t="s">
         <v>1429</v>
-      </c>
-      <c r="B721" s="2" t="s">
-        <v>1430</v>
       </c>
     </row>
     <row r="722" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A722" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B722" s="2" t="s">
         <v>1431</v>
-      </c>
-      <c r="B722" s="2" t="s">
-        <v>1432</v>
       </c>
     </row>
     <row r="723" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A723" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B723" s="2" t="s">
         <v>1433</v>
-      </c>
-      <c r="B723" s="2" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="724" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A724" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B724" s="2" t="s">
         <v>1435</v>
-      </c>
-      <c r="B724" s="2" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="725" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A725" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B725" s="2" t="s">
         <v>1437</v>
-      </c>
-      <c r="B725" s="2" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="726" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A726" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B726" s="2" t="s">
         <v>1439</v>
-      </c>
-      <c r="B726" s="2" t="s">
-        <v>1440</v>
       </c>
     </row>
     <row r="727" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A727" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B727" s="2" t="s">
         <v>1441</v>
-      </c>
-      <c r="B727" s="2" t="s">
-        <v>1442</v>
       </c>
     </row>
     <row r="728" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A728" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B728" s="2" t="s">
         <v>1443</v>
-      </c>
-      <c r="B728" s="2" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="729" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A729" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B729" s="2" t="s">
         <v>1445</v>
-      </c>
-      <c r="B729" s="2" t="s">
-        <v>1446</v>
       </c>
     </row>
     <row r="730" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A730" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B730" s="2" t="s">
         <v>1447</v>
-      </c>
-      <c r="B730" s="2" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="731" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A731" s="2" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B731" s="2" t="s">
         <v>1449</v>
-      </c>
-      <c r="B731" s="2" t="s">
-        <v>1450</v>
       </c>
     </row>
     <row r="732" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A732" s="2" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B732" s="2" t="s">
         <v>1451</v>
-      </c>
-      <c r="B732" s="2" t="s">
-        <v>1452</v>
       </c>
     </row>
     <row r="733" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A733" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B733" s="2" t="s">
         <v>1453</v>
-      </c>
-      <c r="B733" s="2" t="s">
-        <v>1454</v>
       </c>
     </row>
     <row r="734" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A734" s="2" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B734" s="2" t="s">
         <v>1455</v>
-      </c>
-      <c r="B734" s="2" t="s">
-        <v>1456</v>
       </c>
     </row>
     <row r="735" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A735" s="2" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B735" s="2" t="s">
         <v>1457</v>
-      </c>
-      <c r="B735" s="2" t="s">
-        <v>1458</v>
       </c>
     </row>
     <row r="736" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A736" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B736" s="2" t="s">
         <v>1459</v>
-      </c>
-      <c r="B736" s="2" t="s">
-        <v>1460</v>
       </c>
     </row>
     <row r="737" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A737" s="2" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B737" s="2" t="s">
         <v>1461</v>
-      </c>
-      <c r="B737" s="2" t="s">
-        <v>1462</v>
       </c>
     </row>
     <row r="738" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A738" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B738" s="2" t="s">
         <v>1463</v>
-      </c>
-      <c r="B738" s="2" t="s">
-        <v>1464</v>
       </c>
     </row>
     <row r="739" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A739" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B739" s="2" t="s">
         <v>1465</v>
-      </c>
-      <c r="B739" s="2" t="s">
-        <v>1466</v>
       </c>
     </row>
     <row r="740" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A740" s="2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B740" s="2" t="s">
         <v>1467</v>
-      </c>
-      <c r="B740" s="2" t="s">
-        <v>1468</v>
       </c>
     </row>
     <row r="741" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A741" s="2" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B741" s="2" t="s">
         <v>1469</v>
-      </c>
-      <c r="B741" s="2" t="s">
-        <v>1470</v>
       </c>
     </row>
     <row r="742" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A742" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B742" s="2" t="s">
         <v>1471</v>
-      </c>
-      <c r="B742" s="2" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="743" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A743" s="2" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B743" s="2" t="s">
         <v>1473</v>
-      </c>
-      <c r="B743" s="2" t="s">
-        <v>1474</v>
       </c>
     </row>
     <row r="744" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A744" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B744" s="2" t="s">
         <v>1475</v>
-      </c>
-      <c r="B744" s="2" t="s">
-        <v>1476</v>
       </c>
     </row>
     <row r="745" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A745" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B745" s="2" t="s">
         <v>1477</v>
-      </c>
-      <c r="B745" s="2" t="s">
-        <v>1478</v>
       </c>
     </row>
     <row r="746" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A746" s="2" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B746" s="2" t="s">
         <v>1479</v>
-      </c>
-      <c r="B746" s="2" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="747" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A747" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B747" s="2" t="s">
         <v>1481</v>
-      </c>
-      <c r="B747" s="2" t="s">
-        <v>1482</v>
       </c>
     </row>
     <row r="748" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A748" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B748" s="2" t="s">
         <v>1483</v>
-      </c>
-      <c r="B748" s="2" t="s">
-        <v>1484</v>
       </c>
     </row>
     <row r="749" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A749" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B749" s="2" t="s">
         <v>1485</v>
-      </c>
-      <c r="B749" s="2" t="s">
-        <v>1486</v>
       </c>
     </row>
     <row r="750" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A750" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B750" s="2" t="s">
         <v>1487</v>
-      </c>
-      <c r="B750" s="2" t="s">
-        <v>1488</v>
       </c>
     </row>
     <row r="751" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A751" s="2" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B751" s="2" t="s">
         <v>1489</v>
-      </c>
-      <c r="B751" s="2" t="s">
-        <v>1490</v>
       </c>
     </row>
     <row r="752" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A752" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B752" s="2" t="s">
         <v>1491</v>
-      </c>
-      <c r="B752" s="2" t="s">
-        <v>1492</v>
       </c>
     </row>
     <row r="753" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A753" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B753" s="2" t="s">
         <v>1493</v>
-      </c>
-      <c r="B753" s="2" t="s">
-        <v>1494</v>
       </c>
     </row>
     <row r="754" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A754" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B754" s="2" t="s">
         <v>1495</v>
-      </c>
-      <c r="B754" s="2" t="s">
-        <v>1496</v>
       </c>
     </row>
     <row r="755" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A755" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B755" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="B755" s="2" t="s">
-        <v>1498</v>
       </c>
     </row>
     <row r="756" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A756" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B756" s="2" t="s">
         <v>1499</v>
-      </c>
-      <c r="B756" s="2" t="s">
-        <v>1500</v>
       </c>
     </row>
     <row r="757" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A757" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B757" s="2" t="s">
         <v>1501</v>
-      </c>
-      <c r="B757" s="2" t="s">
-        <v>1502</v>
       </c>
     </row>
     <row r="758" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A758" s="2" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B758" s="2" t="s">
         <v>1503</v>
-      </c>
-      <c r="B758" s="2" t="s">
-        <v>1504</v>
       </c>
     </row>
     <row r="759" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A759" s="2" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B759" s="2" t="s">
         <v>1505</v>
-      </c>
-      <c r="B759" s="2" t="s">
-        <v>1506</v>
       </c>
     </row>
     <row r="760" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A760" s="2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B760" s="2" t="s">
         <v>1507</v>
-      </c>
-      <c r="B760" s="2" t="s">
-        <v>1508</v>
       </c>
     </row>
     <row r="761" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A761" s="2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B761" s="2" t="s">
         <v>1509</v>
-      </c>
-      <c r="B761" s="2" t="s">
-        <v>1510</v>
       </c>
     </row>
     <row r="762" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A762" s="2" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B762" s="2" t="s">
         <v>1511</v>
-      </c>
-      <c r="B762" s="2" t="s">
-        <v>1512</v>
       </c>
     </row>
     <row r="763" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A763" s="2" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B763" s="2" t="s">
         <v>1513</v>
-      </c>
-      <c r="B763" s="2" t="s">
-        <v>1514</v>
       </c>
     </row>
     <row r="764" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A764" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B764" s="2" t="s">
         <v>1515</v>
-      </c>
-      <c r="B764" s="2" t="s">
-        <v>1516</v>
       </c>
     </row>
     <row r="765" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A765" s="2" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B765" s="2" t="s">
         <v>1517</v>
-      </c>
-      <c r="B765" s="2" t="s">
-        <v>1518</v>
       </c>
     </row>
     <row r="766" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A766" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B766" s="2" t="s">
         <v>1519</v>
-      </c>
-      <c r="B766" s="2" t="s">
-        <v>1520</v>
       </c>
     </row>
     <row r="767" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A767" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B767" s="2" t="s">
         <v>1521</v>
-      </c>
-      <c r="B767" s="2" t="s">
-        <v>1522</v>
       </c>
     </row>
     <row r="768" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A768" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B768" s="2" t="s">
         <v>1523</v>
-      </c>
-      <c r="B768" s="2" t="s">
-        <v>1524</v>
       </c>
     </row>
     <row r="769" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A769" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B769" s="2" t="s">
         <v>1525</v>
-      </c>
-      <c r="B769" s="2" t="s">
-        <v>1526</v>
       </c>
     </row>
     <row r="770" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A770" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B770" s="2" t="s">
         <v>1527</v>
-      </c>
-      <c r="B770" s="2" t="s">
-        <v>1528</v>
       </c>
     </row>
     <row r="771" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A771" s="2" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B771" s="2" t="s">
         <v>1529</v>
-      </c>
-      <c r="B771" s="2" t="s">
-        <v>1530</v>
       </c>
     </row>
     <row r="772" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A772" s="2" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B772" s="2" t="s">
         <v>1531</v>
-      </c>
-      <c r="B772" s="2" t="s">
-        <v>1532</v>
       </c>
     </row>
     <row r="773" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A773" s="2" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B773" s="2" t="s">
         <v>1533</v>
-      </c>
-      <c r="B773" s="2" t="s">
-        <v>1534</v>
       </c>
     </row>
     <row r="774" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A774" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B774" s="2" t="s">
         <v>1535</v>
-      </c>
-      <c r="B774" s="2" t="s">
-        <v>1536</v>
       </c>
     </row>
     <row r="775" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A775" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B775" s="2" t="s">
         <v>1537</v>
-      </c>
-      <c r="B775" s="2" t="s">
-        <v>1538</v>
       </c>
     </row>
     <row r="776" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A776" s="2" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B776" s="2" t="s">
         <v>1539</v>
-      </c>
-      <c r="B776" s="2" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="777" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A777" s="2" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B777" s="2" t="s">
         <v>1541</v>
-      </c>
-      <c r="B777" s="2" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="778" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A778" s="2" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B778" s="2" t="s">
         <v>1543</v>
-      </c>
-      <c r="B778" s="2" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="779" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A779" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B779" s="2" t="s">
         <v>1545</v>
-      </c>
-      <c r="B779" s="2" t="s">
-        <v>1546</v>
       </c>
     </row>
     <row r="780" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A780" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B780" s="2" t="s">
         <v>1547</v>
-      </c>
-      <c r="B780" s="2" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="781" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A781" s="2" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B781" s="2" t="s">
         <v>1549</v>
-      </c>
-      <c r="B781" s="2" t="s">
-        <v>1550</v>
       </c>
     </row>
     <row r="782" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A782" s="2" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B782" s="2" t="s">
         <v>1551</v>
-      </c>
-      <c r="B782" s="2" t="s">
-        <v>1552</v>
       </c>
     </row>
     <row r="783" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A783" s="2" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B783" s="2" t="s">
         <v>1553</v>
-      </c>
-      <c r="B783" s="2" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="784" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A784" s="2" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B784" s="2" t="s">
         <v>1555</v>
-      </c>
-      <c r="B784" s="2" t="s">
-        <v>1556</v>
       </c>
     </row>
     <row r="785" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A785" s="2" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B785" s="2" t="s">
         <v>1557</v>
-      </c>
-      <c r="B785" s="2" t="s">
-        <v>1558</v>
       </c>
     </row>
     <row r="786" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A786" s="2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B786" s="2" t="s">
         <v>1559</v>
-      </c>
-      <c r="B786" s="2" t="s">
-        <v>1560</v>
       </c>
     </row>
     <row r="787" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A787" s="2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B787" s="2" t="s">
         <v>1561</v>
-      </c>
-      <c r="B787" s="2" t="s">
-        <v>1562</v>
       </c>
     </row>
     <row r="788" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A788" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B788" s="2" t="s">
         <v>1563</v>
-      </c>
-      <c r="B788" s="2" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="789" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A789" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B789" s="2" t="s">
         <v>1565</v>
-      </c>
-      <c r="B789" s="2" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="790" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A790" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B790" s="2" t="s">
         <v>1567</v>
-      </c>
-      <c r="B790" s="2" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="791" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A791" s="2" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B791" s="2" t="s">
         <v>1569</v>
-      </c>
-      <c r="B791" s="2" t="s">
-        <v>1570</v>
       </c>
     </row>
     <row r="792" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A792" s="2" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B792" s="2" t="s">
         <v>1571</v>
-      </c>
-      <c r="B792" s="2" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="793" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A793" s="2" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B793" s="2" t="s">
         <v>1573</v>
-      </c>
-      <c r="B793" s="2" t="s">
-        <v>1574</v>
       </c>
     </row>
     <row r="794" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A794" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B794" s="2" t="s">
         <v>1575</v>
-      </c>
-      <c r="B794" s="2" t="s">
-        <v>1576</v>
       </c>
     </row>
     <row r="795" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A795" s="2" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B795" s="2" t="s">
         <v>1577</v>
-      </c>
-      <c r="B795" s="2" t="s">
-        <v>1578</v>
       </c>
     </row>
     <row r="796" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A796" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B796" s="2" t="s">
         <v>1579</v>
-      </c>
-      <c r="B796" s="2" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="797" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A797" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B797" s="2" t="s">
         <v>1581</v>
-      </c>
-      <c r="B797" s="2" t="s">
-        <v>1582</v>
       </c>
     </row>
     <row r="798" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A798" s="2" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B798" s="2" t="s">
         <v>1583</v>
-      </c>
-      <c r="B798" s="2" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="799" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A799" s="2" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B799" s="2" t="s">
         <v>1585</v>
-      </c>
-      <c r="B799" s="2" t="s">
-        <v>1586</v>
       </c>
     </row>
     <row r="800" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A800" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B800" s="2" t="s">
         <v>1587</v>
-      </c>
-      <c r="B800" s="2" t="s">
-        <v>1588</v>
       </c>
     </row>
     <row r="801" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A801" s="2" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B801" s="2" t="s">
         <v>1589</v>
-      </c>
-      <c r="B801" s="2" t="s">
-        <v>1590</v>
       </c>
     </row>
     <row r="802" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A802" s="2" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B802" s="2" t="s">
         <v>1591</v>
-      </c>
-      <c r="B802" s="2" t="s">
-        <v>1592</v>
       </c>
     </row>
     <row r="803" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A803" s="2" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B803" s="2" t="s">
         <v>1593</v>
-      </c>
-      <c r="B803" s="2" t="s">
-        <v>1594</v>
       </c>
     </row>
     <row r="804" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A804" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B804" s="2" t="s">
         <v>1595</v>
-      </c>
-      <c r="B804" s="2" t="s">
-        <v>1596</v>
       </c>
     </row>
     <row r="805" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A805" s="2" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B805" s="2" t="s">
         <v>1597</v>
-      </c>
-      <c r="B805" s="2" t="s">
-        <v>1598</v>
       </c>
     </row>
     <row r="806" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A806" s="2" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B806" s="2" t="s">
         <v>1599</v>
-      </c>
-      <c r="B806" s="2" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="807" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A807" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B807" s="2" t="s">
         <v>1601</v>
-      </c>
-      <c r="B807" s="2" t="s">
-        <v>1602</v>
       </c>
     </row>
     <row r="808" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A808" s="2" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B808" s="2" t="s">
         <v>1603</v>
-      </c>
-      <c r="B808" s="2" t="s">
-        <v>1604</v>
       </c>
     </row>
     <row r="809" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A809" s="2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B809" s="2" t="s">
         <v>1605</v>
-      </c>
-      <c r="B809" s="2" t="s">
-        <v>1606</v>
       </c>
     </row>
     <row r="810" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A810" s="2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B810" s="2" t="s">
         <v>1607</v>
-      </c>
-      <c r="B810" s="2" t="s">
-        <v>1608</v>
       </c>
     </row>
     <row r="811" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A811" s="2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B811" s="2" t="s">
         <v>1609</v>
-      </c>
-      <c r="B811" s="2" t="s">
-        <v>1610</v>
       </c>
     </row>
     <row r="812" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A812" s="2" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B812" s="2" t="s">
         <v>1611</v>
-      </c>
-      <c r="B812" s="2" t="s">
-        <v>1612</v>
       </c>
     </row>
     <row r="813" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A813" s="2" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B813" s="2" t="s">
         <v>1613</v>
-      </c>
-      <c r="B813" s="2" t="s">
-        <v>1614</v>
       </c>
     </row>
     <row r="814" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A814" s="2" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B814" s="2" t="s">
         <v>1615</v>
-      </c>
-      <c r="B814" s="2" t="s">
-        <v>1616</v>
       </c>
     </row>
     <row r="815" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A815" s="2" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B815" s="2" t="s">
         <v>1617</v>
-      </c>
-      <c r="B815" s="2" t="s">
-        <v>1618</v>
       </c>
     </row>
     <row r="816" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A816" s="2" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B816" s="2" t="s">
         <v>1619</v>
-      </c>
-      <c r="B816" s="2" t="s">
-        <v>1620</v>
       </c>
     </row>
     <row r="817" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A817" s="2" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B817" s="2" t="s">
         <v>1621</v>
-      </c>
-      <c r="B817" s="2" t="s">
-        <v>1622</v>
       </c>
     </row>
     <row r="818" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A818" s="2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B818" s="2" t="s">
         <v>1623</v>
-      </c>
-      <c r="B818" s="2" t="s">
-        <v>1624</v>
       </c>
     </row>
     <row r="819" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A819" s="2" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B819" s="2" t="s">
         <v>1625</v>
-      </c>
-      <c r="B819" s="2" t="s">
-        <v>1626</v>
       </c>
     </row>
     <row r="820" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A820" s="2" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B820" s="2" t="s">
         <v>1627</v>
-      </c>
-      <c r="B820" s="2" t="s">
-        <v>1628</v>
       </c>
     </row>
     <row r="821" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A821" s="2" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B821" s="2" t="s">
         <v>1629</v>
-      </c>
-      <c r="B821" s="2" t="s">
-        <v>1630</v>
       </c>
     </row>
     <row r="822" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A822" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B822" s="2" t="s">
         <v>1631</v>
-      </c>
-      <c r="B822" s="2" t="s">
-        <v>1632</v>
       </c>
     </row>
     <row r="823" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A823" s="2" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B823" s="2" t="s">
         <v>1633</v>
-      </c>
-      <c r="B823" s="2" t="s">
-        <v>1634</v>
       </c>
     </row>
     <row r="824" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A824" s="2" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B824" s="2" t="s">
         <v>1635</v>
-      </c>
-      <c r="B824" s="2" t="s">
-        <v>1636</v>
       </c>
     </row>
     <row r="825" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A825" s="2" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B825" s="2" t="s">
         <v>1637</v>
-      </c>
-      <c r="B825" s="2" t="s">
-        <v>1638</v>
       </c>
     </row>
     <row r="826" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A826" s="2" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B826" s="2" t="s">
         <v>1639</v>
-      </c>
-      <c r="B826" s="2" t="s">
-        <v>1640</v>
       </c>
     </row>
     <row r="827" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A827" s="2" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B827" s="2" t="s">
         <v>1641</v>
-      </c>
-      <c r="B827" s="2" t="s">
-        <v>1642</v>
       </c>
     </row>
     <row r="828" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A828" s="2" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B828" s="2" t="s">
         <v>1643</v>
-      </c>
-      <c r="B828" s="2" t="s">
-        <v>1644</v>
       </c>
     </row>
     <row r="829" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A829" s="2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B829" s="2" t="s">
         <v>1645</v>
-      </c>
-      <c r="B829" s="2" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="830" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A830" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B830" s="2" t="s">
         <v>1647</v>
-      </c>
-      <c r="B830" s="2" t="s">
-        <v>1648</v>
       </c>
     </row>
     <row r="831" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A831" s="2" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B831" s="2" t="s">
         <v>1649</v>
-      </c>
-      <c r="B831" s="2" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="832" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A832" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B832" s="2" t="s">
         <v>1651</v>
-      </c>
-      <c r="B832" s="2" t="s">
-        <v>1652</v>
       </c>
     </row>
     <row r="833" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A833" s="2" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B833" s="2" t="s">
         <v>1653</v>
-      </c>
-      <c r="B833" s="2" t="s">
-        <v>1654</v>
       </c>
     </row>
     <row r="834" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A834" s="2" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B834" s="2" t="s">
         <v>1655</v>
-      </c>
-      <c r="B834" s="2" t="s">
-        <v>1656</v>
       </c>
     </row>
     <row r="835" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A835" s="2" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B835" s="2" t="s">
         <v>1657</v>
-      </c>
-      <c r="B835" s="2" t="s">
-        <v>1658</v>
       </c>
     </row>
     <row r="836" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A836" s="2" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B836" s="2" t="s">
         <v>1659</v>
-      </c>
-      <c r="B836" s="2" t="s">
-        <v>1660</v>
       </c>
     </row>
     <row r="837" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A837" s="2" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B837" s="2" t="s">
         <v>1661</v>
-      </c>
-      <c r="B837" s="2" t="s">
-        <v>1662</v>
       </c>
     </row>
     <row r="838" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A838" s="2" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B838" s="2" t="s">
         <v>1663</v>
-      </c>
-      <c r="B838" s="2" t="s">
-        <v>1664</v>
       </c>
     </row>
     <row r="839" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A839" s="2" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B839" s="2" t="s">
         <v>1665</v>
-      </c>
-      <c r="B839" s="2" t="s">
-        <v>1666</v>
       </c>
     </row>
     <row r="840" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A840" s="2" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B840" s="2" t="s">
         <v>1667</v>
-      </c>
-      <c r="B840" s="2" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="841" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A841" s="2" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B841" s="2" t="s">
         <v>1669</v>
-      </c>
-      <c r="B841" s="2" t="s">
-        <v>1670</v>
       </c>
     </row>
     <row r="842" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A842" s="2" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B842" s="2" t="s">
         <v>1671</v>
-      </c>
-      <c r="B842" s="2" t="s">
-        <v>1672</v>
       </c>
     </row>
     <row r="843" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A843" s="2" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B843" s="2" t="s">
         <v>1673</v>
-      </c>
-      <c r="B843" s="2" t="s">
-        <v>1674</v>
       </c>
     </row>
     <row r="844" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A844" s="2" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B844" s="2" t="s">
         <v>1675</v>
-      </c>
-      <c r="B844" s="2" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="845" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A845" s="2" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B845" s="2" t="s">
         <v>1677</v>
-      </c>
-      <c r="B845" s="2" t="s">
-        <v>1678</v>
       </c>
     </row>
     <row r="846" spans="1:2" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A846" s="2" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B846" s="2" t="s">
         <v>1679</v>
-      </c>
-      <c r="B846" s="2" t="s">
-        <v>1680</v>
       </c>
     </row>
     <row r="847" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A847" s="2" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B847" s="2" t="s">
         <v>1681</v>
-      </c>
-      <c r="B847" s="2" t="s">
-        <v>1682</v>
       </c>
     </row>
     <row r="848" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A848" s="2" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B848" s="2" t="s">
         <v>1683</v>
-      </c>
-      <c r="B848" s="2" t="s">
-        <v>1684</v>
       </c>
     </row>
     <row r="849" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A849" s="2" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B849" s="2" t="s">
         <v>1685</v>
-      </c>
-      <c r="B849" s="2" t="s">
-        <v>1686</v>
       </c>
     </row>
     <row r="850" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A850" s="2" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B850" s="2" t="s">
         <v>1687</v>
-      </c>
-      <c r="B850" s="2" t="s">
-        <v>1688</v>
       </c>
     </row>
     <row r="851" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A851" s="2" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B851" s="2" t="s">
         <v>1689</v>
-      </c>
-      <c r="B851" s="2" t="s">
-        <v>1690</v>
       </c>
     </row>
     <row r="852" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A852" s="2" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B852" s="2" t="s">
         <v>1691</v>
-      </c>
-      <c r="B852" s="2" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="853" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A853" s="2" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B853" s="2" t="s">
         <v>1693</v>
-      </c>
-      <c r="B853" s="2" t="s">
-        <v>1694</v>
       </c>
     </row>
     <row r="854" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A854" s="2" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B854" s="2" t="s">
         <v>1695</v>
-      </c>
-      <c r="B854" s="2" t="s">
-        <v>1696</v>
       </c>
     </row>
     <row r="855" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A855" s="2" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B855" s="2" t="s">
         <v>1697</v>
-      </c>
-      <c r="B855" s="2" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="856" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A856" s="2" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B856" s="2" t="s">
         <v>1699</v>
-      </c>
-      <c r="B856" s="2" t="s">
-        <v>1700</v>
       </c>
     </row>
     <row r="857" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A857" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B857" s="2" t="s">
         <v>1701</v>
-      </c>
-      <c r="B857" s="2" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="858" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A858" s="2" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B858" s="2" t="s">
         <v>1703</v>
-      </c>
-      <c r="B858" s="2" t="s">
-        <v>1704</v>
       </c>
     </row>
     <row r="859" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A859" s="2" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B859" s="2" t="s">
         <v>1705</v>
-      </c>
-      <c r="B859" s="2" t="s">
-        <v>1706</v>
       </c>
     </row>
     <row r="860" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A860" s="2" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B860" s="2" t="s">
         <v>1707</v>
-      </c>
-      <c r="B860" s="2" t="s">
-        <v>1708</v>
       </c>
     </row>
     <row r="861" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A861" s="2" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B861" s="2" t="s">
         <v>1709</v>
-      </c>
-      <c r="B861" s="2" t="s">
-        <v>1710</v>
       </c>
     </row>
     <row r="862" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A862" s="2" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B862" s="2" t="s">
         <v>1711</v>
-      </c>
-      <c r="B862" s="2" t="s">
-        <v>1712</v>
       </c>
     </row>
     <row r="863" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A863" s="2" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B863" s="2" t="s">
         <v>1713</v>
-      </c>
-      <c r="B863" s="2" t="s">
-        <v>1714</v>
       </c>
     </row>
     <row r="864" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A864" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B864" s="2" t="s">
         <v>1715</v>
-      </c>
-      <c r="B864" s="2" t="s">
-        <v>1716</v>
       </c>
     </row>
     <row r="865" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A865" s="2" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B865" s="2" t="s">
         <v>1717</v>
-      </c>
-      <c r="B865" s="2" t="s">
-        <v>1718</v>
       </c>
     </row>
     <row r="866" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A866" s="2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B866" s="2" t="s">
         <v>1719</v>
-      </c>
-      <c r="B866" s="2" t="s">
-        <v>1720</v>
       </c>
     </row>
     <row r="867" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A867" s="2" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B867" s="2" t="s">
         <v>1721</v>
-      </c>
-      <c r="B867" s="2" t="s">
-        <v>1722</v>
       </c>
     </row>
     <row r="868" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A868" s="2" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B868" s="2" t="s">
         <v>1723</v>
-      </c>
-      <c r="B868" s="2" t="s">
-        <v>1724</v>
       </c>
     </row>
     <row r="869" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A869" s="2" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B869" s="2" t="s">
         <v>1725</v>
-      </c>
-      <c r="B869" s="2" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="870" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A870" s="2" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B870" s="2" t="s">
         <v>1727</v>
-      </c>
-      <c r="B870" s="2" t="s">
-        <v>1728</v>
       </c>
     </row>
     <row r="871" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A871" s="2" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B871" s="2" t="s">
         <v>1729</v>
-      </c>
-      <c r="B871" s="2" t="s">
-        <v>1730</v>
       </c>
     </row>
     <row r="872" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A872" s="2" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B872" s="2" t="s">
         <v>1731</v>
-      </c>
-      <c r="B872" s="2" t="s">
-        <v>1732</v>
       </c>
     </row>
     <row r="873" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A873" s="2" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B873" s="2" t="s">
         <v>1733</v>
-      </c>
-      <c r="B873" s="2" t="s">
-        <v>1734</v>
       </c>
     </row>
     <row r="874" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A874" s="2" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B874" s="2" t="s">
         <v>1735</v>
-      </c>
-      <c r="B874" s="2" t="s">
-        <v>1736</v>
       </c>
     </row>
     <row r="875" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A875" s="2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B875" s="2" t="s">
         <v>1737</v>
-      </c>
-      <c r="B875" s="2" t="s">
-        <v>1738</v>
       </c>
     </row>
     <row r="876" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A876" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B876" s="2" t="s">
         <v>1739</v>
-      </c>
-      <c r="B876" s="2" t="s">
-        <v>1740</v>
       </c>
     </row>
     <row r="877" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A877" s="2" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B877" s="2" t="s">
         <v>1741</v>
-      </c>
-      <c r="B877" s="2" t="s">
-        <v>1742</v>
       </c>
     </row>
     <row r="878" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A878" s="2" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B878" s="2" t="s">
         <v>1743</v>
-      </c>
-      <c r="B878" s="2" t="s">
-        <v>1744</v>
       </c>
     </row>
     <row r="879" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A879" s="2" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B879" s="2" t="s">
         <v>1745</v>
-      </c>
-      <c r="B879" s="2" t="s">
-        <v>1746</v>
       </c>
     </row>
     <row r="880" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A880" s="2" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B880" s="2" t="s">
         <v>1747</v>
-      </c>
-      <c r="B880" s="2" t="s">
-        <v>1748</v>
       </c>
     </row>
     <row r="881" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A881" s="2" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B881" s="2" t="s">
         <v>1749</v>
-      </c>
-      <c r="B881" s="2" t="s">
-        <v>1750</v>
       </c>
     </row>
     <row r="882" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A882" s="2" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B882" s="2" t="s">
         <v>1751</v>
-      </c>
-      <c r="B882" s="2" t="s">
-        <v>1752</v>
       </c>
     </row>
     <row r="883" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A883" s="2" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B883" s="2" t="s">
         <v>1753</v>
-      </c>
-      <c r="B883" s="2" t="s">
-        <v>1754</v>
       </c>
     </row>
     <row r="884" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A884" s="2" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B884" s="2" t="s">
         <v>1755</v>
-      </c>
-      <c r="B884" s="2" t="s">
-        <v>1756</v>
       </c>
     </row>
     <row r="885" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A885" s="2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B885" s="2" t="s">
         <v>1757</v>
-      </c>
-      <c r="B885" s="2" t="s">
-        <v>1758</v>
       </c>
     </row>
     <row r="886" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A886" s="2" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B886" s="2" t="s">
         <v>1759</v>
-      </c>
-      <c r="B886" s="2" t="s">
-        <v>1760</v>
       </c>
     </row>
     <row r="887" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A887" s="2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B887" s="2" t="s">
         <v>1761</v>
-      </c>
-      <c r="B887" s="2" t="s">
-        <v>1762</v>
       </c>
     </row>
     <row r="888" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A888" s="2" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B888" s="2" t="s">
         <v>1763</v>
-      </c>
-      <c r="B888" s="2" t="s">
-        <v>1764</v>
       </c>
     </row>
     <row r="889" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A889" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B889" s="2" t="s">
         <v>1765</v>
-      </c>
-      <c r="B889" s="2" t="s">
-        <v>1766</v>
       </c>
     </row>
     <row r="890" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A890" s="2" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B890" s="2" t="s">
         <v>1767</v>
-      </c>
-      <c r="B890" s="2" t="s">
-        <v>1768</v>
       </c>
     </row>
     <row r="891" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A891" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B891" s="2" t="s">
         <v>1769</v>
-      </c>
-      <c r="B891" s="2" t="s">
-        <v>1770</v>
       </c>
     </row>
     <row r="892" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A892" s="2" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B892" s="2" t="s">
         <v>1771</v>
-      </c>
-      <c r="B892" s="2" t="s">
-        <v>1772</v>
       </c>
     </row>
     <row r="893" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A893" s="2" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B893" s="2" t="s">
         <v>1773</v>
-      </c>
-      <c r="B893" s="2" t="s">
-        <v>1774</v>
       </c>
     </row>
     <row r="894" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A894" s="2" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B894" s="2" t="s">
         <v>1775</v>
-      </c>
-      <c r="B894" s="2" t="s">
-        <v>1776</v>
       </c>
     </row>
     <row r="895" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A895" s="2" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B895" s="2" t="s">
         <v>1777</v>
-      </c>
-      <c r="B895" s="2" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="896" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A896" s="2" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B896" s="2" t="s">
         <v>1779</v>
-      </c>
-      <c r="B896" s="2" t="s">
-        <v>1780</v>
       </c>
     </row>
     <row r="897" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A897" s="2" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B897" s="2" t="s">
         <v>1781</v>
-      </c>
-      <c r="B897" s="2" t="s">
-        <v>1782</v>
       </c>
     </row>
     <row r="898" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A898" s="2" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B898" s="2" t="s">
         <v>1783</v>
-      </c>
-      <c r="B898" s="2" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="899" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A899" s="2" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B899" s="2" t="s">
         <v>1785</v>
-      </c>
-      <c r="B899" s="2" t="s">
-        <v>1786</v>
       </c>
     </row>
     <row r="900" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A900" s="2" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B900" s="2" t="s">
         <v>1787</v>
-      </c>
-      <c r="B900" s="2" t="s">
-        <v>1788</v>
       </c>
     </row>
     <row r="901" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A901" s="2" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B901" s="2" t="s">
         <v>1789</v>
-      </c>
-      <c r="B901" s="2" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="902" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A902" s="2" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B902" s="2" t="s">
         <v>1791</v>
-      </c>
-      <c r="B902" s="2" t="s">
-        <v>1792</v>
       </c>
     </row>
     <row r="903" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A903" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B903" s="2" t="s">
         <v>1793</v>
-      </c>
-      <c r="B903" s="2" t="s">
-        <v>1794</v>
       </c>
     </row>
     <row r="904" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A904" s="2" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B904" s="2" t="s">
         <v>1795</v>
-      </c>
-      <c r="B904" s="2" t="s">
-        <v>1796</v>
       </c>
     </row>
     <row r="905" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A905" s="2" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B905" s="2" t="s">
         <v>1797</v>
-      </c>
-      <c r="B905" s="2" t="s">
-        <v>1798</v>
       </c>
     </row>
     <row r="906" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A906" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B906" s="2" t="s">
         <v>1799</v>
-      </c>
-      <c r="B906" s="2" t="s">
-        <v>1800</v>
       </c>
     </row>
     <row r="907" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A907" s="2" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B907" s="2" t="s">
         <v>1801</v>
-      </c>
-      <c r="B907" s="2" t="s">
-        <v>1802</v>
       </c>
     </row>
     <row r="908" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A908" s="2" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B908" s="2" t="s">
         <v>1803</v>
-      </c>
-      <c r="B908" s="2" t="s">
-        <v>1804</v>
       </c>
     </row>
     <row r="909" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A909" s="2" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B909" s="2" t="s">
         <v>1805</v>
-      </c>
-      <c r="B909" s="2" t="s">
-        <v>1806</v>
       </c>
     </row>
     <row r="910" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A910" s="2" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B910" s="2" t="s">
         <v>1807</v>
-      </c>
-      <c r="B910" s="2" t="s">
-        <v>1808</v>
       </c>
     </row>
     <row r="911" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A911" s="2" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B911" s="2" t="s">
         <v>1809</v>
-      </c>
-      <c r="B911" s="2" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="912" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A912" s="2" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B912" s="2" t="s">
         <v>1811</v>
-      </c>
-      <c r="B912" s="2" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="913" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A913" s="2" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B913" s="2" t="s">
         <v>1813</v>
-      </c>
-      <c r="B913" s="2" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="914" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A914" s="2" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B914" s="2" t="s">
         <v>1815</v>
-      </c>
-      <c r="B914" s="2" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="915" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A915" s="2" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B915" s="2" t="s">
         <v>1817</v>
-      </c>
-      <c r="B915" s="2" t="s">
-        <v>1818</v>
       </c>
     </row>
     <row r="916" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A916" s="2" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B916" s="2" t="s">
         <v>1819</v>
-      </c>
-      <c r="B916" s="2" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="917" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A917" s="2" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B917" s="2" t="s">
         <v>1821</v>
-      </c>
-      <c r="B917" s="2" t="s">
-        <v>1822</v>
       </c>
     </row>
     <row r="918" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A918" s="2" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B918" s="2" t="s">
         <v>1823</v>
-      </c>
-      <c r="B918" s="2" t="s">
-        <v>1824</v>
       </c>
     </row>
     <row r="919" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A919" s="2" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B919" s="2" t="s">
         <v>1825</v>
-      </c>
-      <c r="B919" s="2" t="s">
-        <v>1826</v>
       </c>
     </row>
     <row r="920" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A920" s="2" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B920" s="2" t="s">
         <v>1827</v>
-      </c>
-      <c r="B920" s="2" t="s">
-        <v>1828</v>
       </c>
     </row>
     <row r="921" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A921" s="2" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B921" s="2" t="s">
         <v>1829</v>
-      </c>
-      <c r="B921" s="2" t="s">
-        <v>1830</v>
       </c>
     </row>
     <row r="922" spans="1:2" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A922" s="2" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B922" s="2" t="s">
         <v>1831</v>
-      </c>
-      <c r="B922" s="2" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="923" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A923" s="2" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B923" s="2" t="s">
         <v>1833</v>
-      </c>
-      <c r="B923" s="2" t="s">
-        <v>1834</v>
       </c>
     </row>
     <row r="924" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A924" s="2" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B924" s="2" t="s">
         <v>1835</v>
-      </c>
-      <c r="B924" s="2" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="925" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A925" s="2" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B925" s="2" t="s">
         <v>1837</v>
-      </c>
-      <c r="B925" s="2" t="s">
-        <v>1838</v>
       </c>
     </row>
     <row r="926" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A926" s="2" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B926" s="2" t="s">
         <v>1839</v>
-      </c>
-      <c r="B926" s="2" t="s">
-        <v>1840</v>
       </c>
     </row>
     <row r="927" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A927" s="2" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B927" s="2" t="s">
         <v>1841</v>
-      </c>
-      <c r="B927" s="2" t="s">
-        <v>1842</v>
       </c>
     </row>
     <row r="928" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A928" s="2" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B928" s="2" t="s">
         <v>1843</v>
-      </c>
-      <c r="B928" s="2" t="s">
-        <v>1844</v>
       </c>
     </row>
     <row r="929" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A929" s="2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B929" s="2" t="s">
         <v>1845</v>
-      </c>
-      <c r="B929" s="2" t="s">
-        <v>1846</v>
       </c>
     </row>
     <row r="930" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A930" s="2" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B930" s="2" t="s">
         <v>1847</v>
-      </c>
-      <c r="B930" s="2" t="s">
-        <v>1848</v>
       </c>
     </row>
     <row r="931" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A931" s="2" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B931" s="2" t="s">
         <v>1849</v>
-      </c>
-      <c r="B931" s="2" t="s">
-        <v>1850</v>
       </c>
     </row>
     <row r="932" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A932" s="2" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B932" s="2" t="s">
         <v>1851</v>
-      </c>
-      <c r="B932" s="2" t="s">
-        <v>1852</v>
       </c>
     </row>
     <row r="933" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A933" s="2" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B933" s="2" t="s">
         <v>1853</v>
-      </c>
-      <c r="B933" s="2" t="s">
-        <v>1854</v>
       </c>
     </row>
     <row r="934" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A934" s="2" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B934" s="2" t="s">
         <v>1855</v>
-      </c>
-      <c r="B934" s="2" t="s">
-        <v>1856</v>
       </c>
     </row>
     <row r="935" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A935" s="2" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B935" s="2" t="s">
         <v>1857</v>
-      </c>
-      <c r="B935" s="2" t="s">
-        <v>1858</v>
       </c>
     </row>
     <row r="936" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A936" s="2" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B936" s="2" t="s">
         <v>1859</v>
-      </c>
-      <c r="B936" s="2" t="s">
-        <v>1860</v>
       </c>
     </row>
     <row r="937" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A937" s="2" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B937" s="2" t="s">
         <v>1861</v>
-      </c>
-      <c r="B937" s="2" t="s">
-        <v>1862</v>
       </c>
     </row>
     <row r="938" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A938" s="2" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B938" s="2" t="s">
         <v>1863</v>
-      </c>
-      <c r="B938" s="2" t="s">
-        <v>1864</v>
       </c>
     </row>
     <row r="939" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A939" s="2" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B939" s="2" t="s">
         <v>1865</v>
-      </c>
-      <c r="B939" s="2" t="s">
-        <v>1866</v>
       </c>
     </row>
     <row r="940" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A940" s="2" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B940" s="2" t="s">
         <v>1867</v>
-      </c>
-      <c r="B940" s="2" t="s">
-        <v>1868</v>
       </c>
     </row>
     <row r="941" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A941" s="2" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B941" s="2" t="s">
         <v>1869</v>
-      </c>
-      <c r="B941" s="2" t="s">
-        <v>1870</v>
       </c>
     </row>
     <row r="942" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A942" s="2" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B942" s="2" t="s">
         <v>1871</v>
-      </c>
-      <c r="B942" s="2" t="s">
-        <v>1872</v>
       </c>
     </row>
     <row r="943" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A943" s="2" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B943" s="2" t="s">
         <v>1873</v>
-      </c>
-      <c r="B943" s="2" t="s">
-        <v>1874</v>
       </c>
     </row>
     <row r="944" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A944" s="2" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B944" s="2" t="s">
         <v>1875</v>
-      </c>
-      <c r="B944" s="2" t="s">
-        <v>1876</v>
       </c>
     </row>
     <row r="945" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A945" s="2" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B945" s="2" t="s">
         <v>1877</v>
-      </c>
-      <c r="B945" s="2" t="s">
-        <v>1878</v>
       </c>
     </row>
     <row r="946" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A946" s="2" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B946" s="2" t="s">
         <v>1879</v>
-      </c>
-      <c r="B946" s="2" t="s">
-        <v>1880</v>
       </c>
     </row>
     <row r="947" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A947" s="2" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B947" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B947" s="2" t="s">
-        <v>1882</v>
       </c>
     </row>
     <row r="948" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A948" s="2" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B948" s="2" t="s">
         <v>1883</v>
-      </c>
-      <c r="B948" s="2" t="s">
-        <v>1884</v>
       </c>
     </row>
     <row r="949" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A949" s="2" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B949" s="2" t="s">
         <v>1885</v>
-      </c>
-      <c r="B949" s="2" t="s">
-        <v>1886</v>
       </c>
     </row>
     <row r="950" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A950" s="2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B950" s="2" t="s">
         <v>1887</v>
-      </c>
-      <c r="B950" s="2" t="s">
-        <v>1888</v>
       </c>
     </row>
     <row r="951" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A951" s="2" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B951" s="2" t="s">
         <v>1889</v>
-      </c>
-      <c r="B951" s="2" t="s">
-        <v>1890</v>
       </c>
     </row>
     <row r="952" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A952" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B952" s="2" t="s">
         <v>1891</v>
-      </c>
-      <c r="B952" s="2" t="s">
-        <v>1892</v>
       </c>
     </row>
     <row r="953" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A953" s="2" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B953" s="2" t="s">
         <v>1893</v>
-      </c>
-      <c r="B953" s="2" t="s">
-        <v>1894</v>
       </c>
     </row>
     <row r="954" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A954" s="2" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B954" s="2" t="s">
         <v>1895</v>
-      </c>
-      <c r="B954" s="2" t="s">
-        <v>1896</v>
       </c>
     </row>
     <row r="955" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A955" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B955" s="2" t="s">
         <v>1897</v>
-      </c>
-      <c r="B955" s="2" t="s">
-        <v>1898</v>
       </c>
     </row>
     <row r="956" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A956" s="2" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B956" s="2" t="s">
         <v>1899</v>
-      </c>
-      <c r="B956" s="2" t="s">
-        <v>1900</v>
       </c>
     </row>
     <row r="957" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A957" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B957" s="2" t="s">
         <v>1901</v>
-      </c>
-      <c r="B957" s="2" t="s">
-        <v>1902</v>
       </c>
     </row>
     <row r="958" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A958" s="2" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B958" s="2" t="s">
         <v>1903</v>
-      </c>
-      <c r="B958" s="2" t="s">
-        <v>1904</v>
       </c>
     </row>
     <row r="959" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A959" s="2" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B959" s="2" t="s">
         <v>1905</v>
-      </c>
-      <c r="B959" s="2" t="s">
-        <v>1906</v>
       </c>
     </row>
     <row r="960" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A960" s="2" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B960" s="2" t="s">
         <v>1907</v>
-      </c>
-      <c r="B960" s="2" t="s">
-        <v>1908</v>
       </c>
     </row>
     <row r="961" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A961" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B961" s="2" t="s">
         <v>1909</v>
-      </c>
-      <c r="B961" s="2" t="s">
-        <v>1910</v>
       </c>
     </row>
     <row r="962" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A962" s="2" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B962" s="2" t="s">
         <v>1911</v>
-      </c>
-      <c r="B962" s="2" t="s">
-        <v>1912</v>
       </c>
     </row>
     <row r="963" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A963" s="2" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B963" s="2" t="s">
         <v>1913</v>
-      </c>
-      <c r="B963" s="2" t="s">
-        <v>1914</v>
       </c>
     </row>
     <row r="964" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A964" s="2" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B964" s="2" t="s">
         <v>1915</v>
-      </c>
-      <c r="B964" s="2" t="s">
-        <v>1916</v>
       </c>
     </row>
     <row r="965" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A965" s="2" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B965" s="2" t="s">
         <v>1917</v>
-      </c>
-      <c r="B965" s="2" t="s">
-        <v>1918</v>
       </c>
     </row>
     <row r="966" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A966" s="2" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B966" s="2" t="s">
         <v>1919</v>
-      </c>
-      <c r="B966" s="2" t="s">
-        <v>1920</v>
       </c>
     </row>
     <row r="967" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A967" s="2" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B967" s="2" t="s">
         <v>1921</v>
-      </c>
-      <c r="B967" s="2" t="s">
-        <v>1922</v>
       </c>
     </row>
     <row r="968" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A968" s="2" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B968" s="2" t="s">
         <v>1923</v>
-      </c>
-      <c r="B968" s="2" t="s">
-        <v>1924</v>
       </c>
     </row>
     <row r="969" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A969" s="2" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B969" s="2" t="s">
         <v>1925</v>
-      </c>
-      <c r="B969" s="2" t="s">
-        <v>1926</v>
       </c>
     </row>
     <row r="970" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A970" s="2" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B970" s="2" t="s">
         <v>1927</v>
-      </c>
-      <c r="B970" s="2" t="s">
-        <v>1928</v>
       </c>
     </row>
     <row r="971" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A971" s="2" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B971" s="2" t="s">
         <v>1929</v>
-      </c>
-      <c r="B971" s="2" t="s">
-        <v>1930</v>
       </c>
     </row>
     <row r="972" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A972" s="2" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B972" s="2" t="s">
         <v>1931</v>
-      </c>
-      <c r="B972" s="2" t="s">
-        <v>1932</v>
       </c>
     </row>
     <row r="973" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A973" s="2" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B973" s="2" t="s">
         <v>1933</v>
-      </c>
-      <c r="B973" s="2" t="s">
-        <v>1934</v>
       </c>
     </row>
     <row r="974" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A974" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B974" s="2" t="s">
         <v>1935</v>
-      </c>
-      <c r="B974" s="2" t="s">
-        <v>1936</v>
       </c>
     </row>
     <row r="975" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A975" s="2" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B975" s="2" t="s">
         <v>1937</v>
-      </c>
-      <c r="B975" s="2" t="s">
-        <v>1938</v>
       </c>
     </row>
     <row r="976" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A976" s="2" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B976" s="2" t="s">
         <v>1939</v>
-      </c>
-      <c r="B976" s="2" t="s">
-        <v>1940</v>
       </c>
     </row>
     <row r="977" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A977" s="2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B977" s="2" t="s">
         <v>1941</v>
-      </c>
-      <c r="B977" s="2" t="s">
-        <v>1942</v>
       </c>
     </row>
     <row r="978" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A978" s="2" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B978" s="2" t="s">
         <v>1943</v>
-      </c>
-      <c r="B978" s="2" t="s">
-        <v>1944</v>
       </c>
     </row>
     <row r="979" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A979" s="2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B979" s="2" t="s">
         <v>1945</v>
-      </c>
-      <c r="B979" s="2" t="s">
-        <v>1946</v>
       </c>
     </row>
     <row r="980" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A980" s="2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B980" s="2" t="s">
         <v>1947</v>
-      </c>
-      <c r="B980" s="2" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="981" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A981" s="2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B981" s="2" t="s">
         <v>1949</v>
-      </c>
-      <c r="B981" s="2" t="s">
-        <v>1950</v>
       </c>
     </row>
     <row r="982" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A982" s="2" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B982" s="2" t="s">
         <v>1951</v>
-      </c>
-      <c r="B982" s="2" t="s">
-        <v>1952</v>
       </c>
     </row>
     <row r="983" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A983" s="2" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B983" s="2" t="s">
         <v>1953</v>
-      </c>
-      <c r="B983" s="2" t="s">
-        <v>1954</v>
       </c>
     </row>
     <row r="984" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A984" s="2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B984" s="2" t="s">
         <v>1955</v>
-      </c>
-      <c r="B984" s="2" t="s">
-        <v>1956</v>
       </c>
     </row>
     <row r="985" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A985" s="2" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B985" s="2" t="s">
         <v>1957</v>
-      </c>
-      <c r="B985" s="2" t="s">
-        <v>1958</v>
       </c>
     </row>
     <row r="986" spans="1:2" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A986" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B986" s="2" t="s">
         <v>1959</v>
-      </c>
-      <c r="B986" s="2" t="s">
-        <v>1960</v>
       </c>
     </row>
     <row r="987" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A987" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B987" s="2" t="s">
         <v>1961</v>
-      </c>
-      <c r="B987" s="2" t="s">
-        <v>1962</v>
       </c>
     </row>
     <row r="988" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A988" s="2" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B988" s="2" t="s">
         <v>1963</v>
-      </c>
-      <c r="B988" s="2" t="s">
-        <v>1964</v>
       </c>
     </row>
     <row r="989" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A989" s="2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B989" s="2" t="s">
         <v>1965</v>
-      </c>
-      <c r="B989" s="2" t="s">
-        <v>1966</v>
       </c>
     </row>
     <row r="990" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A990" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B990" s="2" t="s">
         <v>1967</v>
-      </c>
-      <c r="B990" s="2" t="s">
-        <v>1968</v>
       </c>
     </row>
     <row r="991" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A991" s="2" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B991" s="2" t="s">
         <v>1969</v>
-      </c>
-      <c r="B991" s="2" t="s">
-        <v>1970</v>
       </c>
     </row>
     <row r="992" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A992" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B992" s="2" t="s">
         <v>1971</v>
-      </c>
-      <c r="B992" s="2" t="s">
-        <v>1972</v>
       </c>
     </row>
     <row r="993" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A993" s="2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B993" s="2" t="s">
         <v>1973</v>
-      </c>
-      <c r="B993" s="2" t="s">
-        <v>1974</v>
       </c>
     </row>
     <row r="994" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A994" s="2" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B994" s="2" t="s">
         <v>1975</v>
-      </c>
-      <c r="B994" s="2" t="s">
-        <v>1976</v>
       </c>
     </row>
     <row r="995" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A995" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B995" s="2" t="s">
         <v>1977</v>
-      </c>
-      <c r="B995" s="2" t="s">
-        <v>1978</v>
       </c>
     </row>
     <row r="996" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A996" s="2" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B996" s="2" t="s">
         <v>1979</v>
-      </c>
-      <c r="B996" s="2" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="997" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A997" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B997" s="2" t="s">
         <v>1981</v>
-      </c>
-      <c r="B997" s="2" t="s">
-        <v>1982</v>
       </c>
     </row>
     <row r="998" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A998" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B998" s="2" t="s">
         <v>1983</v>
-      </c>
-      <c r="B998" s="2" t="s">
-        <v>1984</v>
       </c>
     </row>
     <row r="999" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A999" s="2" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B999" s="2" t="s">
         <v>1985</v>
-      </c>
-      <c r="B999" s="2" t="s">
-        <v>1986</v>
       </c>
     </row>
     <row r="1000" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1000" s="2" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B1000" s="2" t="s">
         <v>1987</v>
-      </c>
-      <c r="B1000" s="2" t="s">
-        <v>1988</v>
       </c>
     </row>
     <row r="1001" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1001" s="2" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B1001" s="2" t="s">
         <v>1989</v>
-      </c>
-      <c r="B1001" s="2" t="s">
-        <v>1990</v>
       </c>
     </row>
     <row r="1002" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1002" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B1002" s="2" t="s">
         <v>1991</v>
-      </c>
-      <c r="B1002" s="2" t="s">
-        <v>1992</v>
       </c>
     </row>
     <row r="1003" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1003" s="2" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B1003" s="2" t="s">
         <v>1993</v>
-      </c>
-      <c r="B1003" s="2" t="s">
-        <v>1994</v>
       </c>
     </row>
     <row r="1004" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1004" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B1004" s="2" t="s">
         <v>1995</v>
-      </c>
-      <c r="B1004" s="2" t="s">
-        <v>1996</v>
       </c>
     </row>
     <row r="1005" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1005" s="2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B1005" s="2" t="s">
         <v>1997</v>
-      </c>
-      <c r="B1005" s="2" t="s">
-        <v>1998</v>
       </c>
     </row>
     <row r="1006" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1006" s="2" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B1006" s="2" t="s">
         <v>1999</v>
-      </c>
-      <c r="B1006" s="2" t="s">
-        <v>2000</v>
       </c>
     </row>
     <row r="1007" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1007" s="2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1007" s="2" t="s">
         <v>2001</v>
-      </c>
-      <c r="B1007" s="2" t="s">
-        <v>2002</v>
       </c>
     </row>
     <row r="1008" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1008" s="2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B1008" s="2" t="s">
         <v>2003</v>
-      </c>
-      <c r="B1008" s="2" t="s">
-        <v>2004</v>
       </c>
     </row>
     <row r="1009" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1009" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B1009" s="2" t="s">
         <v>2005</v>
-      </c>
-      <c r="B1009" s="2" t="s">
-        <v>2006</v>
       </c>
     </row>
     <row r="1010" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1010" s="2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B1010" s="2" t="s">
         <v>2007</v>
-      </c>
-      <c r="B1010" s="2" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="1011" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1011" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B1011" s="2" t="s">
         <v>2009</v>
-      </c>
-      <c r="B1011" s="2" t="s">
-        <v>2010</v>
       </c>
     </row>
     <row r="1012" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1012" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B1012" s="2" t="s">
         <v>2011</v>
-      </c>
-      <c r="B1012" s="2" t="s">
-        <v>2012</v>
       </c>
     </row>
     <row r="1013" spans="1:2" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1013" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B1013" s="2" t="s">
         <v>2013</v>
-      </c>
-      <c r="B1013" s="2" t="s">
-        <v>2014</v>
       </c>
     </row>
     <row r="1014" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1014" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B1014" s="2" t="s">
         <v>2015</v>
-      </c>
-      <c r="B1014" s="2" t="s">
-        <v>2016</v>
       </c>
     </row>
     <row r="1015" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1015" s="2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B1015" s="2" t="s">
         <v>2017</v>
-      </c>
-      <c r="B1015" s="2" t="s">
-        <v>2018</v>
       </c>
     </row>
     <row r="1016" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1016" s="2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B1016" s="2" t="s">
         <v>2019</v>
-      </c>
-      <c r="B1016" s="2" t="s">
-        <v>2020</v>
       </c>
     </row>
     <row r="1017" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1017" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B1017" s="2" t="s">
         <v>2021</v>
-      </c>
-      <c r="B1017" s="2" t="s">
-        <v>2022</v>
       </c>
     </row>
     <row r="1018" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1018" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B1018" s="2" t="s">
         <v>2023</v>
-      </c>
-      <c r="B1018" s="2" t="s">
-        <v>2024</v>
       </c>
     </row>
     <row r="1019" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1019" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B1019" s="2" t="s">
         <v>2025</v>
-      </c>
-      <c r="B1019" s="2" t="s">
-        <v>2026</v>
       </c>
     </row>
     <row r="1020" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1020" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B1020" s="2" t="s">
         <v>2027</v>
-      </c>
-      <c r="B1020" s="2" t="s">
-        <v>2028</v>
       </c>
     </row>
     <row r="1021" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1021" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B1021" s="2" t="s">
         <v>2029</v>
-      </c>
-      <c r="B1021" s="2" t="s">
-        <v>2030</v>
       </c>
     </row>
     <row r="1022" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1022" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B1022" s="2" t="s">
         <v>2031</v>
-      </c>
-      <c r="B1022" s="2" t="s">
-        <v>2032</v>
       </c>
     </row>
     <row r="1023" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1023" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B1023" s="2" t="s">
         <v>2033</v>
-      </c>
-      <c r="B1023" s="2" t="s">
-        <v>2034</v>
       </c>
     </row>
     <row r="1024" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1024" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B1024" s="2" t="s">
         <v>2035</v>
-      </c>
-      <c r="B1024" s="2" t="s">
-        <v>2036</v>
       </c>
     </row>
     <row r="1025" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1025" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B1025" s="2" t="s">
         <v>2037</v>
-      </c>
-      <c r="B1025" s="2" t="s">
-        <v>2038</v>
       </c>
     </row>
     <row r="1026" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1026" s="2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B1026" s="2" t="s">
         <v>2039</v>
-      </c>
-      <c r="B1026" s="2" t="s">
-        <v>2040</v>
       </c>
     </row>
     <row r="1027" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1027" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B1027" s="2" t="s">
         <v>2041</v>
-      </c>
-      <c r="B1027" s="2" t="s">
-        <v>2042</v>
       </c>
     </row>
     <row r="1028" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1028" s="2" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B1028" s="2" t="s">
         <v>2043</v>
-      </c>
-      <c r="B1028" s="2" t="s">
-        <v>2044</v>
       </c>
     </row>
     <row r="1029" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1029" s="2" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B1029" s="2" t="s">
         <v>2045</v>
-      </c>
-      <c r="B1029" s="2" t="s">
-        <v>2046</v>
       </c>
     </row>
     <row r="1030" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1030" s="2" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B1030" s="2" t="s">
         <v>2047</v>
-      </c>
-      <c r="B1030" s="2" t="s">
-        <v>2048</v>
       </c>
     </row>
     <row r="1031" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1031" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B1031" s="2" t="s">
         <v>2049</v>
-      </c>
-      <c r="B1031" s="2" t="s">
-        <v>2050</v>
       </c>
     </row>
     <row r="1032" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1032" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B1032" s="2" t="s">
         <v>2051</v>
-      </c>
-      <c r="B1032" s="2" t="s">
-        <v>2052</v>
       </c>
     </row>
     <row r="1033" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1033" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B1033" s="2" t="s">
         <v>2053</v>
-      </c>
-      <c r="B1033" s="2" t="s">
-        <v>2054</v>
       </c>
     </row>
     <row r="1034" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1034" s="2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1034" s="2" t="s">
         <v>2055</v>
-      </c>
-      <c r="B1034" s="2" t="s">
-        <v>2056</v>
       </c>
     </row>
     <row r="1035" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1035" s="2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="B1035" s="2" t="s">
         <v>2057</v>
-      </c>
-      <c r="B1035" s="2" t="s">
-        <v>2058</v>
       </c>
     </row>
     <row r="1036" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1036" s="2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="B1036" s="2" t="s">
         <v>2059</v>
-      </c>
-      <c r="B1036" s="2" t="s">
-        <v>2060</v>
       </c>
     </row>
     <row r="1037" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1037" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B1037" s="2" t="s">
         <v>2061</v>
-      </c>
-      <c r="B1037" s="2" t="s">
-        <v>2062</v>
       </c>
     </row>
     <row r="1038" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1038" s="2" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B1038" s="2" t="s">
         <v>2063</v>
-      </c>
-      <c r="B1038" s="2" t="s">
-        <v>2064</v>
       </c>
     </row>
     <row r="1039" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1039" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B1039" s="2" t="s">
         <v>2065</v>
-      </c>
-      <c r="B1039" s="2" t="s">
-        <v>2066</v>
       </c>
     </row>
     <row r="1040" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1040" s="2" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B1040" s="2" t="s">
         <v>2067</v>
-      </c>
-      <c r="B1040" s="2" t="s">
-        <v>2068</v>
       </c>
     </row>
     <row r="1041" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1041" s="2" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B1041" s="2" t="s">
         <v>2069</v>
-      </c>
-      <c r="B1041" s="2" t="s">
-        <v>2070</v>
       </c>
     </row>
     <row r="1042" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1042" s="2" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B1042" s="2" t="s">
         <v>2071</v>
-      </c>
-      <c r="B1042" s="2" t="s">
-        <v>2072</v>
       </c>
     </row>
     <row r="1043" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1043" s="2" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B1043" s="2" t="s">
         <v>2073</v>
-      </c>
-      <c r="B1043" s="2" t="s">
-        <v>2074</v>
       </c>
     </row>
     <row r="1044" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1044" s="2" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B1044" s="2" t="s">
         <v>305</v>
@@ -15285,338 +15285,338 @@
     </row>
     <row r="1045" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1045" s="2" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1045" s="2" t="s">
         <v>2076</v>
-      </c>
-      <c r="B1045" s="2" t="s">
-        <v>2077</v>
       </c>
     </row>
     <row r="1046" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1046" s="2" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B1046" s="2" t="s">
         <v>2078</v>
-      </c>
-      <c r="B1046" s="2" t="s">
-        <v>2079</v>
       </c>
     </row>
     <row r="1047" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1047" s="2" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B1047" s="2" t="s">
         <v>2080</v>
-      </c>
-      <c r="B1047" s="2" t="s">
-        <v>2081</v>
       </c>
     </row>
     <row r="1048" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1048" s="2" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B1048" s="2" t="s">
         <v>2082</v>
-      </c>
-      <c r="B1048" s="2" t="s">
-        <v>2083</v>
       </c>
     </row>
     <row r="1049" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1049" s="2" t="s">
+        <v>2083</v>
+      </c>
+      <c r="B1049" s="2" t="s">
         <v>2084</v>
-      </c>
-      <c r="B1049" s="2" t="s">
-        <v>2085</v>
       </c>
     </row>
     <row r="1050" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1050" s="2" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B1050" s="2" t="s">
         <v>2086</v>
-      </c>
-      <c r="B1050" s="2" t="s">
-        <v>2087</v>
       </c>
     </row>
     <row r="1051" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1051" s="2" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B1051" s="2" t="s">
         <v>2088</v>
-      </c>
-      <c r="B1051" s="2" t="s">
-        <v>2089</v>
       </c>
     </row>
     <row r="1052" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1052" s="2" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B1052" s="2" t="s">
         <v>2090</v>
-      </c>
-      <c r="B1052" s="2" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="1053" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1053" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B1053" s="2" t="s">
         <v>2092</v>
-      </c>
-      <c r="B1053" s="2" t="s">
-        <v>2093</v>
       </c>
     </row>
     <row r="1054" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1054" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B1054" s="2" t="s">
         <v>2094</v>
-      </c>
-      <c r="B1054" s="2" t="s">
-        <v>2095</v>
       </c>
     </row>
     <row r="1055" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1055" s="2" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B1055" s="2" t="s">
         <v>2096</v>
-      </c>
-      <c r="B1055" s="2" t="s">
-        <v>2097</v>
       </c>
     </row>
     <row r="1056" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1056" s="2" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B1056" s="2" t="s">
         <v>2098</v>
-      </c>
-      <c r="B1056" s="2" t="s">
-        <v>2099</v>
       </c>
     </row>
     <row r="1057" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1057" s="2" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B1057" s="2" t="s">
         <v>2100</v>
-      </c>
-      <c r="B1057" s="2" t="s">
-        <v>2101</v>
       </c>
     </row>
     <row r="1058" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1058" s="2" t="s">
+        <v>2101</v>
+      </c>
+      <c r="B1058" s="2" t="s">
         <v>2102</v>
-      </c>
-      <c r="B1058" s="2" t="s">
-        <v>2103</v>
       </c>
     </row>
     <row r="1059" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1059" s="2" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B1059" s="2" t="s">
         <v>2104</v>
-      </c>
-      <c r="B1059" s="2" t="s">
-        <v>2105</v>
       </c>
     </row>
     <row r="1060" spans="1:2" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1060" s="2" t="s">
+        <v>2105</v>
+      </c>
+      <c r="B1060" s="2" t="s">
         <v>2106</v>
-      </c>
-      <c r="B1060" s="2" t="s">
-        <v>2107</v>
       </c>
     </row>
     <row r="1061" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1061" s="2" t="s">
+        <v>2107</v>
+      </c>
+      <c r="B1061" s="2" t="s">
         <v>2108</v>
-      </c>
-      <c r="B1061" s="2" t="s">
-        <v>2109</v>
       </c>
     </row>
     <row r="1062" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1062" s="2" t="s">
+        <v>2109</v>
+      </c>
+      <c r="B1062" s="2" t="s">
         <v>2110</v>
-      </c>
-      <c r="B1062" s="2" t="s">
-        <v>2111</v>
       </c>
     </row>
     <row r="1063" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1063" s="2" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B1063" s="2" t="s">
         <v>2112</v>
-      </c>
-      <c r="B1063" s="2" t="s">
-        <v>2113</v>
       </c>
     </row>
     <row r="1064" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1064" s="2" t="s">
+        <v>2113</v>
+      </c>
+      <c r="B1064" s="2" t="s">
         <v>2114</v>
-      </c>
-      <c r="B1064" s="2" t="s">
-        <v>2115</v>
       </c>
     </row>
     <row r="1065" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1065" s="2" t="s">
+        <v>2115</v>
+      </c>
+      <c r="B1065" s="2" t="s">
         <v>2116</v>
-      </c>
-      <c r="B1065" s="2" t="s">
-        <v>2117</v>
       </c>
     </row>
     <row r="1066" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1066" s="2" t="s">
+        <v>2117</v>
+      </c>
+      <c r="B1066" s="2" t="s">
         <v>2118</v>
-      </c>
-      <c r="B1066" s="2" t="s">
-        <v>2119</v>
       </c>
     </row>
     <row r="1067" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1067" s="2" t="s">
+        <v>2119</v>
+      </c>
+      <c r="B1067" s="2" t="s">
         <v>2120</v>
-      </c>
-      <c r="B1067" s="2" t="s">
-        <v>2121</v>
       </c>
     </row>
     <row r="1068" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1068" s="2" t="s">
+        <v>2121</v>
+      </c>
+      <c r="B1068" s="2" t="s">
         <v>2122</v>
-      </c>
-      <c r="B1068" s="2" t="s">
-        <v>2123</v>
       </c>
     </row>
     <row r="1069" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1069" s="2" t="s">
+        <v>2123</v>
+      </c>
+      <c r="B1069" s="2" t="s">
         <v>2124</v>
-      </c>
-      <c r="B1069" s="2" t="s">
-        <v>2125</v>
       </c>
     </row>
     <row r="1070" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1070" s="2" t="s">
+        <v>2125</v>
+      </c>
+      <c r="B1070" s="2" t="s">
         <v>2126</v>
-      </c>
-      <c r="B1070" s="2" t="s">
-        <v>2127</v>
       </c>
     </row>
     <row r="1071" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1071" s="2" t="s">
+        <v>2127</v>
+      </c>
+      <c r="B1071" s="2" t="s">
         <v>2128</v>
-      </c>
-      <c r="B1071" s="2" t="s">
-        <v>2129</v>
       </c>
     </row>
     <row r="1072" spans="1:2" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A1072" s="2" t="s">
+        <v>2129</v>
+      </c>
+      <c r="B1072" s="2" t="s">
         <v>2130</v>
-      </c>
-      <c r="B1072" s="2" t="s">
-        <v>2131</v>
       </c>
     </row>
     <row r="1073" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1073" s="2" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B1073" s="2" t="s">
         <v>2132</v>
-      </c>
-      <c r="B1073" s="2" t="s">
-        <v>2133</v>
       </c>
     </row>
     <row r="1074" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1074" s="2" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B1074" s="2" t="s">
         <v>2134</v>
-      </c>
-      <c r="B1074" s="2" t="s">
-        <v>2135</v>
       </c>
     </row>
     <row r="1075" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1075" s="2" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B1075" s="2" t="s">
         <v>2136</v>
-      </c>
-      <c r="B1075" s="2" t="s">
-        <v>2137</v>
       </c>
     </row>
     <row r="1076" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1076" s="2" t="s">
+        <v>2137</v>
+      </c>
+      <c r="B1076" s="2" t="s">
         <v>2138</v>
-      </c>
-      <c r="B1076" s="2" t="s">
-        <v>2139</v>
       </c>
     </row>
     <row r="1077" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1077" s="2" t="s">
+        <v>2139</v>
+      </c>
+      <c r="B1077" s="2" t="s">
         <v>2140</v>
-      </c>
-      <c r="B1077" s="2" t="s">
-        <v>2141</v>
       </c>
     </row>
     <row r="1078" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1078" s="2" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B1078" s="2" t="s">
         <v>2142</v>
-      </c>
-      <c r="B1078" s="2" t="s">
-        <v>2143</v>
       </c>
     </row>
     <row r="1079" spans="1:2" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1079" s="2" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B1079" s="2" t="s">
         <v>2144</v>
-      </c>
-      <c r="B1079" s="2" t="s">
-        <v>2145</v>
       </c>
     </row>
     <row r="1080" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1080" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="B1080" s="2" t="s">
         <v>2146</v>
-      </c>
-      <c r="B1080" s="2" t="s">
-        <v>2147</v>
       </c>
     </row>
     <row r="1081" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1081" s="2" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B1081" s="2" t="s">
         <v>2148</v>
-      </c>
-      <c r="B1081" s="2" t="s">
-        <v>2149</v>
       </c>
     </row>
     <row r="1082" spans="1:2" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1082" s="2" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B1082" s="2" t="s">
         <v>2150</v>
-      </c>
-      <c r="B1082" s="2" t="s">
-        <v>2151</v>
       </c>
     </row>
     <row r="1083" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1083" s="2" t="s">
+        <v>2151</v>
+      </c>
+      <c r="B1083" s="2" t="s">
         <v>2152</v>
-      </c>
-      <c r="B1083" s="2" t="s">
-        <v>2153</v>
       </c>
     </row>
     <row r="1084" spans="1:2" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1084" s="2" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B1084" s="2" t="s">
         <v>2154</v>
-      </c>
-      <c r="B1084" s="2" t="s">
-        <v>2155</v>
       </c>
     </row>
     <row r="1085" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1085" s="2" t="s">
+        <v>2155</v>
+      </c>
+      <c r="B1085" s="2" t="s">
         <v>2156</v>
-      </c>
-      <c r="B1085" s="2" t="s">
-        <v>2157</v>
       </c>
     </row>
     <row r="1086" spans="1:2" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1086" s="2" t="s">
+        <v>2157</v>
+      </c>
+      <c r="B1086" s="2" t="s">
         <v>2158</v>
-      </c>
-      <c r="B1086" s="2" t="s">
-        <v>2159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>